<commit_message>
motchallenge: result MOTA for iou tracker from the provided detections (from DPM model)
</commit_message>
<xml_diff>
--- a/results/MOT16-results.xlsx
+++ b/results/MOT16-results.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adzie\code\deeplens\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8104D87-86E4-4107-A52E-3A7D6FBC4D5D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAD3C5D7-C507-4CB1-91E2-08CEC9B8723B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="18192" windowHeight="12192" activeTab="2" xr2:uid="{EF9591CC-71C4-478A-8487-EA15B85DAC3C}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="18192" windowHeight="12192" activeTab="1" xr2:uid="{EF9591CC-71C4-478A-8487-EA15B85DAC3C}"/>
   </bookViews>
   <sheets>
-    <sheet name="darknet_sort_1" sheetId="1" r:id="rId1"/>
-    <sheet name="darknet_sort_2" sheetId="3" r:id="rId2"/>
-    <sheet name="darknet_sort_3" sheetId="5" r:id="rId3"/>
-    <sheet name="ground_truth" sheetId="2" r:id="rId4"/>
+    <sheet name="ground_truth" sheetId="2" r:id="rId1"/>
+    <sheet name="iou_on_gt_dets" sheetId="7" r:id="rId2"/>
+    <sheet name="darknet_sort_1" sheetId="1" r:id="rId3"/>
+    <sheet name="darknet_sort_2" sheetId="3" r:id="rId4"/>
+    <sheet name="darknet_sort_3" sheetId="5" r:id="rId5"/>
+    <sheet name="darknet_sort_4" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="45">
   <si>
     <t>MOT16-02</t>
   </si>
@@ -157,6 +159,18 @@
   </si>
   <si>
     <t>sort_tracker</t>
+  </si>
+  <si>
+    <t>#_people</t>
+  </si>
+  <si>
+    <t>#_people_per_frame</t>
+  </si>
+  <si>
+    <t>#_objects</t>
+  </si>
+  <si>
+    <t>#_objects_per_frame</t>
   </si>
 </sst>
 </file>
@@ -527,11 +541,808 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F354829-DC5C-43BE-8791-A3024D6061C7}">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="13.05078125" customWidth="1"/>
+    <col min="2" max="2" width="22.26171875" customWidth="1"/>
+    <col min="3" max="3" width="49.68359375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="13.8" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>66</v>
+      </c>
+      <c r="C2">
+        <v>41.088333333333303</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>88</v>
+      </c>
+      <c r="C3">
+        <v>49.861904761904697</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>129</v>
+      </c>
+      <c r="C4">
+        <v>8.5221027479091997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>25</v>
+      </c>
+      <c r="C5">
+        <v>10.0133333333333</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>57</v>
+      </c>
+      <c r="C6">
+        <v>20.938837920489199</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>69</v>
+      </c>
+      <c r="C7">
+        <v>10.1933333333333</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>107</v>
+      </c>
+      <c r="C8">
+        <v>15.2666666666666</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8611D968-EEAD-4617-8B40-E1DBE56A0987}">
+  <dimension ref="A1:R20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="14.15625" customWidth="1"/>
+    <col min="6" max="6" width="5.3671875" customWidth="1"/>
+    <col min="7" max="7" width="12.47265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="1"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N2" t="s">
+        <v>20</v>
+      </c>
+      <c r="O2" t="s">
+        <v>21</v>
+      </c>
+      <c r="P2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>23</v>
+      </c>
+      <c r="R2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>14.4</v>
+      </c>
+      <c r="C3">
+        <v>53.1</v>
+      </c>
+      <c r="D3">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="E3">
+        <v>15.1</v>
+      </c>
+      <c r="F3">
+        <v>96</v>
+      </c>
+      <c r="G3">
+        <v>0.19</v>
+      </c>
+      <c r="H3">
+        <v>54</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
+      </c>
+      <c r="J3">
+        <v>14</v>
+      </c>
+      <c r="K3">
+        <v>38</v>
+      </c>
+      <c r="L3">
+        <v>112</v>
+      </c>
+      <c r="M3">
+        <v>15144</v>
+      </c>
+      <c r="N3">
+        <v>66</v>
+      </c>
+      <c r="O3">
+        <v>85</v>
+      </c>
+      <c r="P3">
+        <v>14.1</v>
+      </c>
+      <c r="Q3">
+        <v>75.900000000000006</v>
+      </c>
+      <c r="R3">
+        <v>14.4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>26.1</v>
+      </c>
+      <c r="C4">
+        <v>52.7</v>
+      </c>
+      <c r="D4">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="E4">
+        <v>31.7</v>
+      </c>
+      <c r="F4">
+        <v>96.5</v>
+      </c>
+      <c r="G4">
+        <v>0.52</v>
+      </c>
+      <c r="H4">
+        <v>83</v>
+      </c>
+      <c r="I4">
+        <v>5</v>
+      </c>
+      <c r="J4">
+        <v>36</v>
+      </c>
+      <c r="K4">
+        <v>42</v>
+      </c>
+      <c r="L4">
+        <v>549</v>
+      </c>
+      <c r="M4">
+        <v>32460</v>
+      </c>
+      <c r="N4">
+        <v>317</v>
+      </c>
+      <c r="O4">
+        <v>335</v>
+      </c>
+      <c r="P4">
+        <v>29.9</v>
+      </c>
+      <c r="Q4">
+        <v>79.7</v>
+      </c>
+      <c r="R4">
+        <v>30.6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>29.8</v>
+      </c>
+      <c r="C5">
+        <v>67.7</v>
+      </c>
+      <c r="D5">
+        <v>19.100000000000001</v>
+      </c>
+      <c r="E5">
+        <v>27.2</v>
+      </c>
+      <c r="F5">
+        <v>96.2</v>
+      </c>
+      <c r="G5">
+        <v>0.09</v>
+      </c>
+      <c r="H5">
+        <v>125</v>
+      </c>
+      <c r="I5">
+        <v>4</v>
+      </c>
+      <c r="J5">
+        <v>42</v>
+      </c>
+      <c r="K5">
+        <v>79</v>
+      </c>
+      <c r="L5">
+        <v>73</v>
+      </c>
+      <c r="M5">
+        <v>4962</v>
+      </c>
+      <c r="N5">
+        <v>49</v>
+      </c>
+      <c r="O5">
+        <v>65</v>
+      </c>
+      <c r="P5">
+        <v>25.4</v>
+      </c>
+      <c r="Q5">
+        <v>77.3</v>
+      </c>
+      <c r="R5">
+        <v>26.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>42.6</v>
+      </c>
+      <c r="C6">
+        <v>65.099999999999994</v>
+      </c>
+      <c r="D6">
+        <v>31.7</v>
+      </c>
+      <c r="E6">
+        <v>46.6</v>
+      </c>
+      <c r="F6">
+        <v>95.8</v>
+      </c>
+      <c r="G6">
+        <v>0.21</v>
+      </c>
+      <c r="H6">
+        <v>25</v>
+      </c>
+      <c r="I6">
+        <v>4</v>
+      </c>
+      <c r="J6">
+        <v>16</v>
+      </c>
+      <c r="K6">
+        <v>5</v>
+      </c>
+      <c r="L6">
+        <v>108</v>
+      </c>
+      <c r="M6">
+        <v>2808</v>
+      </c>
+      <c r="N6">
+        <v>83</v>
+      </c>
+      <c r="O6">
+        <v>101</v>
+      </c>
+      <c r="P6">
+        <v>43</v>
+      </c>
+      <c r="Q6">
+        <v>74.900000000000006</v>
+      </c>
+      <c r="R6">
+        <v>44.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>18.7</v>
+      </c>
+      <c r="C7">
+        <v>42.6</v>
+      </c>
+      <c r="D7">
+        <v>11.9</v>
+      </c>
+      <c r="E7">
+        <v>27.5</v>
+      </c>
+      <c r="F7">
+        <v>98</v>
+      </c>
+      <c r="G7">
+        <v>0.1</v>
+      </c>
+      <c r="H7">
+        <v>54</v>
+      </c>
+      <c r="I7">
+        <v>2</v>
+      </c>
+      <c r="J7">
+        <v>16</v>
+      </c>
+      <c r="K7">
+        <v>36</v>
+      </c>
+      <c r="L7">
+        <v>68</v>
+      </c>
+      <c r="M7">
+        <v>8930</v>
+      </c>
+      <c r="N7">
+        <v>137</v>
+      </c>
+      <c r="O7">
+        <v>150</v>
+      </c>
+      <c r="P7">
+        <v>25.8</v>
+      </c>
+      <c r="Q7">
+        <v>76</v>
+      </c>
+      <c r="R7">
+        <v>26.9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>46.5</v>
+      </c>
+      <c r="C8">
+        <v>70.099999999999994</v>
+      </c>
+      <c r="D8">
+        <v>34.799999999999997</v>
+      </c>
+      <c r="E8">
+        <v>48.4</v>
+      </c>
+      <c r="F8">
+        <v>97.6</v>
+      </c>
+      <c r="G8">
+        <v>0.12</v>
+      </c>
+      <c r="H8">
+        <v>69</v>
+      </c>
+      <c r="I8">
+        <v>6</v>
+      </c>
+      <c r="J8">
+        <v>27</v>
+      </c>
+      <c r="K8">
+        <v>36</v>
+      </c>
+      <c r="L8">
+        <v>107</v>
+      </c>
+      <c r="M8">
+        <v>4734</v>
+      </c>
+      <c r="N8">
+        <v>63</v>
+      </c>
+      <c r="O8">
+        <v>66</v>
+      </c>
+      <c r="P8">
+        <v>46.5</v>
+      </c>
+      <c r="Q8">
+        <v>78.8</v>
+      </c>
+      <c r="R8">
+        <v>47.2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9">
+        <v>11.3</v>
+      </c>
+      <c r="C9">
+        <v>64.7</v>
+      </c>
+      <c r="D9">
+        <v>6.2</v>
+      </c>
+      <c r="E9">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="F9">
+        <v>95.7</v>
+      </c>
+      <c r="G9">
+        <v>0.06</v>
+      </c>
+      <c r="H9">
+        <v>107</v>
+      </c>
+      <c r="I9">
+        <v>2</v>
+      </c>
+      <c r="J9">
+        <v>11</v>
+      </c>
+      <c r="K9">
+        <v>94</v>
+      </c>
+      <c r="L9">
+        <v>47</v>
+      </c>
+      <c r="M9">
+        <v>10398</v>
+      </c>
+      <c r="N9">
+        <v>36</v>
+      </c>
+      <c r="O9">
+        <v>39</v>
+      </c>
+      <c r="P9">
+        <v>8.5</v>
+      </c>
+      <c r="Q9">
+        <v>74.3</v>
+      </c>
+      <c r="R9">
+        <v>8.8000000000000007</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10">
+        <v>25.4</v>
+      </c>
+      <c r="C10">
+        <v>56.4</v>
+      </c>
+      <c r="D10">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="E10">
+        <v>28.1</v>
+      </c>
+      <c r="F10">
+        <v>96.7</v>
+      </c>
+      <c r="G10">
+        <v>0.2</v>
+      </c>
+      <c r="H10">
+        <v>517</v>
+      </c>
+      <c r="I10">
+        <v>25</v>
+      </c>
+      <c r="J10">
+        <v>162</v>
+      </c>
+      <c r="K10">
+        <v>330</v>
+      </c>
+      <c r="L10">
+        <v>1064</v>
+      </c>
+      <c r="M10">
+        <v>79436</v>
+      </c>
+      <c r="N10">
+        <v>751</v>
+      </c>
+      <c r="O10">
+        <v>841</v>
+      </c>
+      <c r="P10" s="2">
+        <v>26.4</v>
+      </c>
+      <c r="Q10">
+        <v>78.099999999999994</v>
+      </c>
+      <c r="R10">
+        <v>27.1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14">
+        <v>93</v>
+      </c>
+      <c r="C14">
+        <v>4.7149999999999999</v>
+      </c>
+      <c r="D14">
+        <v>93</v>
+      </c>
+      <c r="E14">
+        <v>4.7149999999999999</v>
+      </c>
+      <c r="F14">
+        <f>(D14-ground_truth!B2)/ground_truth!B2 * 100</f>
+        <v>40.909090909090914</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15">
+        <v>389</v>
+      </c>
+      <c r="C15">
+        <v>14.9323809523809</v>
+      </c>
+      <c r="D15">
+        <v>389</v>
+      </c>
+      <c r="E15">
+        <v>14.9323809523809</v>
+      </c>
+      <c r="F15">
+        <f>(D15-ground_truth!B3)/ground_truth!B3 * 100</f>
+        <v>342.04545454545456</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16">
+        <v>95</v>
+      </c>
+      <c r="C16">
+        <v>2.42032622333751</v>
+      </c>
+      <c r="D16">
+        <v>95</v>
+      </c>
+      <c r="E16">
+        <v>2.42032622333751</v>
+      </c>
+      <c r="F16">
+        <f>(D16-ground_truth!B4)/ground_truth!B4 * 100</f>
+        <v>-26.356589147286826</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17">
+        <v>106</v>
+      </c>
+      <c r="C17">
+        <v>5.0857142857142801</v>
+      </c>
+      <c r="D17">
+        <v>106</v>
+      </c>
+      <c r="E17">
+        <v>5.0857142857142801</v>
+      </c>
+      <c r="F17">
+        <f>(D17-ground_truth!B5)/ground_truth!B5 * 100</f>
+        <v>324</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18">
+        <v>164</v>
+      </c>
+      <c r="C18">
+        <v>5.28440366972477</v>
+      </c>
+      <c r="D18">
+        <v>164</v>
+      </c>
+      <c r="E18">
+        <v>5.28440366972477</v>
+      </c>
+      <c r="F18">
+        <f>(D18-ground_truth!B6)/ground_truth!B6 * 100</f>
+        <v>187.71929824561403</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19">
+        <v>101</v>
+      </c>
+      <c r="C19">
+        <v>5.0522222222222197</v>
+      </c>
+      <c r="D19">
+        <v>101</v>
+      </c>
+      <c r="E19">
+        <v>5.0522222222222197</v>
+      </c>
+      <c r="F19">
+        <f>(D19-ground_truth!B7)/ground_truth!B7 * 100</f>
+        <v>46.376811594202898</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20">
+        <v>70</v>
+      </c>
+      <c r="C20">
+        <v>1.93827160493827</v>
+      </c>
+      <c r="D20">
+        <v>70</v>
+      </c>
+      <c r="E20">
+        <v>1.93827160493827</v>
+      </c>
+      <c r="F20">
+        <f>(D20-ground_truth!B8)/ground_truth!B8 * 100</f>
+        <v>-34.579439252336449</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{016F5681-380E-497D-A5D0-C78F88FBF6E7}">
   <dimension ref="A1:R20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1275,7 +2086,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9515722-321E-4F21-8A44-93AC984BEED1}">
   <dimension ref="A1:R20"/>
   <sheetViews>
@@ -2021,12 +2832,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62791F90-C7BC-4273-BF71-38B690B0C6D5}">
   <dimension ref="A1:R20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2781,107 +3592,758 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F354829-DC5C-43BE-8791-A3024D6061C7}">
-  <dimension ref="A1:C8"/>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{100D8D13-5042-4D32-870C-476FD1E164DC}">
+  <dimension ref="A1:R20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="13.05078125" customWidth="1"/>
-    <col min="2" max="2" width="22.26171875" customWidth="1"/>
-    <col min="3" max="3" width="49.68359375" customWidth="1"/>
+    <col min="1" max="1" width="14.15625" customWidth="1"/>
+    <col min="7" max="7" width="12.47265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="B1" t="s">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="1"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N2" t="s">
+        <v>20</v>
+      </c>
+      <c r="O2" t="s">
+        <v>21</v>
+      </c>
+      <c r="P2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>23</v>
+      </c>
+      <c r="R2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>15.8</v>
+      </c>
+      <c r="C3">
+        <v>37.299999999999997</v>
+      </c>
+      <c r="D3">
+        <v>10</v>
+      </c>
+      <c r="E3">
+        <v>19.5</v>
+      </c>
+      <c r="F3">
+        <v>72.7</v>
+      </c>
+      <c r="G3">
+        <v>2.17</v>
+      </c>
+      <c r="H3">
+        <v>54</v>
+      </c>
+      <c r="I3">
+        <v>6</v>
+      </c>
+      <c r="J3">
+        <v>12</v>
+      </c>
+      <c r="K3">
+        <v>36</v>
+      </c>
+      <c r="L3">
+        <v>1304</v>
+      </c>
+      <c r="M3">
+        <v>14359</v>
+      </c>
+      <c r="N3">
+        <v>135</v>
+      </c>
+      <c r="O3">
+        <v>116</v>
+      </c>
+      <c r="P3">
+        <v>11.4</v>
+      </c>
+      <c r="Q3">
+        <v>76.8</v>
+      </c>
+      <c r="R3">
+        <v>12.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>24.3</v>
+      </c>
+      <c r="C4">
+        <v>39.799999999999997</v>
+      </c>
+      <c r="D4">
+        <v>17.5</v>
+      </c>
+      <c r="E4">
+        <v>34.200000000000003</v>
+      </c>
+      <c r="F4">
+        <v>77.900000000000006</v>
+      </c>
+      <c r="G4">
+        <v>4.41</v>
+      </c>
+      <c r="H4">
+        <v>83</v>
+      </c>
+      <c r="I4">
+        <v>6</v>
+      </c>
+      <c r="J4">
+        <v>35</v>
+      </c>
+      <c r="K4">
+        <v>42</v>
+      </c>
+      <c r="L4">
+        <v>4630</v>
+      </c>
+      <c r="M4">
+        <v>31278</v>
+      </c>
+      <c r="N4">
+        <v>340</v>
+      </c>
+      <c r="O4">
+        <v>364</v>
+      </c>
+      <c r="P4">
+        <v>23.8</v>
+      </c>
+      <c r="Q4">
+        <v>77.7</v>
+      </c>
+      <c r="R4">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>36.799999999999997</v>
+      </c>
+      <c r="C5">
+        <v>43.9</v>
+      </c>
+      <c r="D5">
+        <v>31.7</v>
+      </c>
+      <c r="E5">
+        <v>51.6</v>
+      </c>
+      <c r="F5">
+        <v>71.400000000000006</v>
+      </c>
+      <c r="G5">
+        <v>1.68</v>
+      </c>
+      <c r="H5">
+        <v>125</v>
+      </c>
+      <c r="I5">
+        <v>9</v>
+      </c>
+      <c r="J5">
+        <v>75</v>
+      </c>
+      <c r="K5">
+        <v>41</v>
+      </c>
+      <c r="L5">
+        <v>1405</v>
+      </c>
+      <c r="M5">
+        <v>3302</v>
+      </c>
+      <c r="N5">
+        <v>209</v>
+      </c>
+      <c r="O5">
+        <v>190</v>
+      </c>
+      <c r="P5">
+        <v>27.9</v>
+      </c>
+      <c r="Q5">
+        <v>74.5</v>
+      </c>
+      <c r="R5">
+        <v>30.9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>35.1</v>
+      </c>
+      <c r="C6">
+        <v>45</v>
+      </c>
+      <c r="D6">
+        <v>28.7</v>
+      </c>
+      <c r="E6">
+        <v>54.4</v>
+      </c>
+      <c r="F6">
+        <v>85.1</v>
+      </c>
+      <c r="G6">
+        <v>0.95</v>
+      </c>
+      <c r="H6">
+        <v>25</v>
+      </c>
+      <c r="I6">
+        <v>6</v>
+      </c>
+      <c r="J6">
+        <v>16</v>
+      </c>
+      <c r="K6">
+        <v>3</v>
+      </c>
+      <c r="L6">
+        <v>501</v>
+      </c>
+      <c r="M6">
+        <v>2398</v>
+      </c>
+      <c r="N6">
+        <v>146</v>
+      </c>
+      <c r="O6">
+        <v>136</v>
+      </c>
+      <c r="P6">
+        <v>42.1</v>
+      </c>
+      <c r="Q6">
+        <v>78.599999999999994</v>
+      </c>
+      <c r="R6">
+        <v>44.8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="C7">
+        <v>36.5</v>
+      </c>
+      <c r="D7">
+        <v>13.8</v>
+      </c>
+      <c r="E7">
+        <v>31.8</v>
+      </c>
+      <c r="F7">
+        <v>84</v>
+      </c>
+      <c r="G7">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="H7">
+        <v>54</v>
+      </c>
+      <c r="I7">
+        <v>6</v>
+      </c>
+      <c r="J7">
+        <v>15</v>
+      </c>
+      <c r="K7">
         <v>33</v>
       </c>
-      <c r="C1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="13.8" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" t="s">
+      <c r="L7">
+        <v>747</v>
+      </c>
+      <c r="M7">
+        <v>8396</v>
+      </c>
+      <c r="N7">
+        <v>170</v>
+      </c>
+      <c r="O7">
+        <v>207</v>
+      </c>
+      <c r="P7">
+        <v>24.4</v>
+      </c>
+      <c r="Q7">
+        <v>76.2</v>
+      </c>
+      <c r="R7">
+        <v>25.8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>36.4</v>
+      </c>
+      <c r="C8">
+        <v>47.5</v>
+      </c>
+      <c r="D8">
+        <v>29.4</v>
+      </c>
+      <c r="E8">
+        <v>55.4</v>
+      </c>
+      <c r="F8">
+        <v>89.5</v>
+      </c>
+      <c r="G8">
+        <v>0.66</v>
+      </c>
+      <c r="H8">
+        <v>69</v>
+      </c>
+      <c r="I8">
+        <v>13</v>
+      </c>
+      <c r="J8">
+        <v>23</v>
+      </c>
+      <c r="K8">
+        <v>33</v>
+      </c>
+      <c r="L8">
+        <v>598</v>
+      </c>
+      <c r="M8">
+        <v>4091</v>
+      </c>
+      <c r="N8">
+        <v>124</v>
+      </c>
+      <c r="O8">
+        <v>104</v>
+      </c>
+      <c r="P8">
+        <v>47.5</v>
+      </c>
+      <c r="Q8">
+        <v>81.900000000000006</v>
+      </c>
+      <c r="R8">
+        <v>48.9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9">
+        <v>14.8</v>
+      </c>
+      <c r="C9">
+        <v>23</v>
+      </c>
+      <c r="D9">
+        <v>10.9</v>
+      </c>
+      <c r="E9">
+        <v>18.5</v>
+      </c>
+      <c r="F9">
+        <v>39.299999999999997</v>
+      </c>
+      <c r="G9">
+        <v>4.37</v>
+      </c>
+      <c r="H9">
+        <v>107</v>
+      </c>
+      <c r="I9">
+        <v>7</v>
+      </c>
+      <c r="J9">
+        <v>25</v>
+      </c>
+      <c r="K9">
+        <v>75</v>
+      </c>
+      <c r="L9">
+        <v>3276</v>
+      </c>
+      <c r="M9">
+        <v>9329</v>
+      </c>
+      <c r="N9">
+        <v>139</v>
+      </c>
+      <c r="O9">
+        <v>165</v>
+      </c>
+      <c r="P9">
+        <v>-11.3</v>
+      </c>
+      <c r="Q9">
+        <v>73.3</v>
+      </c>
+      <c r="R9">
+        <v>-10.1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10">
+        <v>24.3</v>
+      </c>
+      <c r="C10">
+        <v>39.1</v>
+      </c>
+      <c r="D10">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="E10">
+        <v>33.700000000000003</v>
+      </c>
+      <c r="F10">
+        <v>74.900000000000006</v>
+      </c>
+      <c r="G10">
+        <v>2.34</v>
+      </c>
+      <c r="H10">
+        <v>517</v>
+      </c>
+      <c r="I10">
+        <v>53</v>
+      </c>
+      <c r="J10">
+        <v>201</v>
+      </c>
+      <c r="K10">
+        <v>263</v>
+      </c>
+      <c r="L10">
+        <v>12461</v>
+      </c>
+      <c r="M10">
+        <v>73153</v>
+      </c>
+      <c r="N10">
+        <v>1263</v>
+      </c>
+      <c r="O10">
+        <v>1282</v>
+      </c>
+      <c r="P10" s="2">
+        <v>21.3</v>
+      </c>
+      <c r="Q10">
+        <v>77.5</v>
+      </c>
+      <c r="R10">
+        <v>22.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" t="s">
+        <v>30</v>
+      </c>
+      <c r="F13" t="s">
+        <v>31</v>
+      </c>
+      <c r="G13" t="s">
+        <v>32</v>
+      </c>
+      <c r="H13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" t="s">
         <v>0</v>
       </c>
-      <c r="B2">
-        <v>66</v>
-      </c>
-      <c r="C2">
-        <v>41.088333333333303</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" t="s">
+      <c r="B14">
+        <v>0.7</v>
+      </c>
+      <c r="C14">
+        <v>0.6</v>
+      </c>
+      <c r="D14">
         <v>1</v>
       </c>
-      <c r="B3">
-        <v>88</v>
-      </c>
-      <c r="C3">
-        <v>49.861904761904697</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" t="s">
+      <c r="E14">
+        <v>3</v>
+      </c>
+      <c r="F14">
+        <v>209</v>
+      </c>
+      <c r="G14">
+        <v>7.1483333333333299</v>
+      </c>
+      <c r="H14">
+        <f>(F14-ground_truth!B2)/ground_truth!B2 * 100</f>
+        <v>216.66666666666666</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15">
+        <v>0.7</v>
+      </c>
+      <c r="C15">
+        <v>0.6</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>3</v>
+      </c>
+      <c r="F15">
+        <v>511</v>
+      </c>
+      <c r="G15">
+        <v>17.5942857142857</v>
+      </c>
+      <c r="H15">
+        <f>(F15-ground_truth!B3)/ground_truth!B3 * 100</f>
+        <v>480.68181818181819</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" t="s">
         <v>2</v>
       </c>
-      <c r="B4">
-        <v>129</v>
-      </c>
-      <c r="C4">
-        <v>8.5221027479091997</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" t="s">
+      <c r="B16">
+        <v>0.7</v>
+      </c>
+      <c r="C16">
+        <v>0.6</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
         <v>3</v>
       </c>
-      <c r="B5">
-        <v>25</v>
-      </c>
-      <c r="C5">
-        <v>10.0133333333333</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" t="s">
+      <c r="F16">
+        <v>323</v>
+      </c>
+      <c r="G16">
+        <v>4.7479091995221001</v>
+      </c>
+      <c r="H16">
+        <f>(F16-ground_truth!B4)/ground_truth!B4 * 100</f>
+        <v>150.3875968992248</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17">
+        <v>0.7</v>
+      </c>
+      <c r="C17">
+        <v>0.6</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>3</v>
+      </c>
+      <c r="F17">
+        <v>172</v>
+      </c>
+      <c r="G17">
+        <v>6.43619047619047</v>
+      </c>
+      <c r="H17">
+        <f>(F17-ground_truth!B5)/ground_truth!B5 * 100</f>
+        <v>588</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" t="s">
         <v>4</v>
       </c>
-      <c r="B6">
-        <v>57</v>
-      </c>
-      <c r="C6">
-        <v>20.938837920489199</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" t="s">
+      <c r="B18">
+        <v>0.7</v>
+      </c>
+      <c r="C18">
+        <v>0.6</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>3</v>
+      </c>
+      <c r="F18">
+        <v>210</v>
+      </c>
+      <c r="G18">
+        <v>6.6773700305810397</v>
+      </c>
+      <c r="H18">
+        <f>(F18-ground_truth!B6)/ground_truth!B6 * 100</f>
+        <v>268.42105263157896</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" t="s">
         <v>5</v>
       </c>
-      <c r="B7">
-        <v>69</v>
-      </c>
-      <c r="C7">
-        <v>10.1933333333333</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" t="s">
+      <c r="B19">
+        <v>0.7</v>
+      </c>
+      <c r="C19">
+        <v>0.6</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>3</v>
+      </c>
+      <c r="F19">
+        <v>186</v>
+      </c>
+      <c r="G19">
+        <v>6.0255555555555498</v>
+      </c>
+      <c r="H19">
+        <f>(F19-ground_truth!B7)/ground_truth!B7 * 100</f>
+        <v>169.56521739130434</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" t="s">
         <v>6</v>
       </c>
-      <c r="B8">
-        <v>107</v>
-      </c>
-      <c r="C8">
-        <v>15.2666666666666</v>
+      <c r="B20">
+        <v>0.7</v>
+      </c>
+      <c r="C20">
+        <v>0.6</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>3</v>
+      </c>
+      <c r="F20">
+        <v>195</v>
+      </c>
+      <c r="G20">
+        <v>3.2413314840499301</v>
+      </c>
+      <c r="H20">
+        <f>(F20-ground_truth!B8)/ground_truth!B8 * 100</f>
+        <v>82.242990654205599</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
tracking for on-line iou better than the off-line iou, sort is slightly worse, based on ground truth detections
</commit_message>
<xml_diff>
--- a/results/MOT16-results.xlsx
+++ b/results/MOT16-results.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adzie\code\deeplens\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{800BF071-6B82-4311-A3A7-386761FF1D6B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9CB79FF-B544-40DF-BB6F-8537F09F85F8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="18192" windowHeight="12192" activeTab="2" xr2:uid="{EF9591CC-71C4-478A-8487-EA15B85DAC3C}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="18192" windowHeight="12192" firstSheet="1" activeTab="2" xr2:uid="{EF9591CC-71C4-478A-8487-EA15B85DAC3C}"/>
   </bookViews>
   <sheets>
     <sheet name="ground_truth" sheetId="2" r:id="rId1"/>
-    <sheet name="iou_on_gt_dets" sheetId="7" r:id="rId2"/>
-    <sheet name="sort_on_gt_dets" sheetId="8" r:id="rId3"/>
-    <sheet name="darknet_sort_1" sheetId="1" r:id="rId4"/>
-    <sheet name="darknet_sort_2" sheetId="3" r:id="rId5"/>
-    <sheet name="darknet_sort_3" sheetId="5" r:id="rId6"/>
-    <sheet name="darknet_sort_4" sheetId="6" r:id="rId7"/>
+    <sheet name="gt_dets_online_iou" sheetId="9" r:id="rId2"/>
+    <sheet name="gt_dets_offline_iou" sheetId="7" r:id="rId3"/>
+    <sheet name="gt_dets_sort" sheetId="8" r:id="rId4"/>
+    <sheet name="darknet_sort_1" sheetId="1" r:id="rId5"/>
+    <sheet name="darknet_sort_2" sheetId="3" r:id="rId6"/>
+    <sheet name="darknet_sort_3" sheetId="5" r:id="rId7"/>
+    <sheet name="darknet_sort_4" sheetId="6" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="54">
   <si>
     <t>MOT16-02</t>
   </si>
@@ -178,6 +179,27 @@
   </si>
   <si>
     <t>ady@skr-compute1:/local/ady/code/deeplens/benchmarks/motchallenge/res/MOT16/sort_tracker/MOT16_gt__sort_tracker_max_age_1_min_hits_3$</t>
+  </si>
+  <si>
+    <t>sigma_l</t>
+  </si>
+  <si>
+    <t>sigma_h</t>
+  </si>
+  <si>
+    <t>sigma_iou</t>
+  </si>
+  <si>
+    <t>t_min</t>
+  </si>
+  <si>
+    <t>t_max</t>
+  </si>
+  <si>
+    <t>iou_tracker</t>
+  </si>
+  <si>
+    <t>match_labels (should we check the label from the previous state of the track)</t>
   </si>
 </sst>
 </file>
@@ -662,11 +684,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8611D968-EEAD-4617-8B40-E1DBE56A0987}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B611522-1655-46D4-A137-76DD73A801D1}">
   <dimension ref="A1:R20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -740,55 +762,55 @@
         <v>0</v>
       </c>
       <c r="B3">
-        <v>14.4</v>
+        <v>16.399999999999999</v>
       </c>
       <c r="C3">
-        <v>53.1</v>
+        <v>53.8</v>
       </c>
       <c r="D3">
-        <v>8.3000000000000007</v>
+        <v>9.6</v>
       </c>
       <c r="E3">
-        <v>15.1</v>
+        <v>16.600000000000001</v>
       </c>
       <c r="F3">
-        <v>96</v>
+        <v>92.9</v>
       </c>
       <c r="G3">
-        <v>0.19</v>
+        <v>0.38</v>
       </c>
       <c r="H3">
         <v>54</v>
       </c>
       <c r="I3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J3">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K3">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="L3">
-        <v>112</v>
+        <v>226</v>
       </c>
       <c r="M3">
-        <v>15144</v>
+        <v>14864</v>
       </c>
       <c r="N3">
-        <v>66</v>
+        <v>127</v>
       </c>
       <c r="O3">
-        <v>85</v>
+        <v>225</v>
       </c>
       <c r="P3">
-        <v>14.1</v>
+        <v>14.7</v>
       </c>
       <c r="Q3">
-        <v>75.900000000000006</v>
+        <v>75.599999999999994</v>
       </c>
       <c r="R3">
-        <v>14.4</v>
+        <v>15.4</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.55000000000000004">
@@ -796,22 +818,22 @@
         <v>1</v>
       </c>
       <c r="B4">
-        <v>26.1</v>
+        <v>31</v>
       </c>
       <c r="C4">
-        <v>52.7</v>
+        <v>57.6</v>
       </c>
       <c r="D4">
-        <v>17.399999999999999</v>
+        <v>21.2</v>
       </c>
       <c r="E4">
-        <v>31.7</v>
+        <v>34.6</v>
       </c>
       <c r="F4">
-        <v>96.5</v>
+        <v>94</v>
       </c>
       <c r="G4">
-        <v>0.52</v>
+        <v>1.01</v>
       </c>
       <c r="H4">
         <v>83</v>
@@ -820,31 +842,31 @@
         <v>5</v>
       </c>
       <c r="J4">
+        <v>42</v>
+      </c>
+      <c r="K4">
         <v>36</v>
       </c>
-      <c r="K4">
-        <v>42</v>
-      </c>
       <c r="L4">
-        <v>549</v>
+        <v>1058</v>
       </c>
       <c r="M4">
-        <v>32460</v>
+        <v>31114</v>
       </c>
       <c r="N4">
-        <v>317</v>
+        <v>554</v>
       </c>
       <c r="O4">
-        <v>335</v>
+        <v>1114</v>
       </c>
       <c r="P4">
-        <v>29.9</v>
+        <v>31.2</v>
       </c>
       <c r="Q4">
-        <v>79.7</v>
+        <v>79</v>
       </c>
       <c r="R4">
-        <v>30.6</v>
+        <v>32.299999999999997</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.55000000000000004">
@@ -852,55 +874,55 @@
         <v>2</v>
       </c>
       <c r="B5">
-        <v>29.8</v>
+        <v>33.299999999999997</v>
       </c>
       <c r="C5">
-        <v>67.7</v>
+        <v>67</v>
       </c>
       <c r="D5">
-        <v>19.100000000000001</v>
+        <v>22.2</v>
       </c>
       <c r="E5">
-        <v>27.2</v>
+        <v>30.7</v>
       </c>
       <c r="F5">
-        <v>96.2</v>
+        <v>92.6</v>
       </c>
       <c r="G5">
-        <v>0.09</v>
+        <v>0.2</v>
       </c>
       <c r="H5">
         <v>125</v>
       </c>
       <c r="I5">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="J5">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="K5">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="L5">
-        <v>73</v>
+        <v>166</v>
       </c>
       <c r="M5">
-        <v>4962</v>
+        <v>4727</v>
       </c>
       <c r="N5">
-        <v>49</v>
+        <v>110</v>
       </c>
       <c r="O5">
-        <v>65</v>
+        <v>172</v>
       </c>
       <c r="P5">
-        <v>25.4</v>
+        <v>26.6</v>
       </c>
       <c r="Q5">
-        <v>77.3</v>
+        <v>76.5</v>
       </c>
       <c r="R5">
-        <v>26.1</v>
+        <v>28.2</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.55000000000000004">
@@ -908,22 +930,22 @@
         <v>3</v>
       </c>
       <c r="B6">
-        <v>42.6</v>
+        <v>44.3</v>
       </c>
       <c r="C6">
-        <v>65.099999999999994</v>
+        <v>62.5</v>
       </c>
       <c r="D6">
-        <v>31.7</v>
+        <v>34.4</v>
       </c>
       <c r="E6">
-        <v>46.6</v>
+        <v>50</v>
       </c>
       <c r="F6">
-        <v>95.8</v>
+        <v>91.1</v>
       </c>
       <c r="G6">
-        <v>0.21</v>
+        <v>0.49</v>
       </c>
       <c r="H6">
         <v>25</v>
@@ -938,25 +960,25 @@
         <v>5</v>
       </c>
       <c r="L6">
-        <v>108</v>
+        <v>257</v>
       </c>
       <c r="M6">
-        <v>2808</v>
+        <v>2626</v>
       </c>
       <c r="N6">
-        <v>83</v>
+        <v>126</v>
       </c>
       <c r="O6">
-        <v>101</v>
+        <v>202</v>
       </c>
       <c r="P6">
-        <v>43</v>
+        <v>42.8</v>
       </c>
       <c r="Q6">
-        <v>74.900000000000006</v>
+        <v>74.2</v>
       </c>
       <c r="R6">
-        <v>44.5</v>
+        <v>45.1</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.55000000000000004">
@@ -964,55 +986,55 @@
         <v>4</v>
       </c>
       <c r="B7">
-        <v>18.7</v>
+        <v>29.8</v>
       </c>
       <c r="C7">
-        <v>42.6</v>
+        <v>59.1</v>
       </c>
       <c r="D7">
-        <v>11.9</v>
+        <v>19.899999999999999</v>
       </c>
       <c r="E7">
-        <v>27.5</v>
+        <v>31.7</v>
       </c>
       <c r="F7">
-        <v>98</v>
+        <v>94.1</v>
       </c>
       <c r="G7">
-        <v>0.1</v>
+        <v>0.37</v>
       </c>
       <c r="H7">
         <v>54</v>
       </c>
       <c r="I7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J7">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="K7">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="L7">
-        <v>68</v>
+        <v>243</v>
       </c>
       <c r="M7">
-        <v>8930</v>
+        <v>8412</v>
       </c>
       <c r="N7">
-        <v>137</v>
+        <v>181</v>
       </c>
       <c r="O7">
-        <v>150</v>
+        <v>453</v>
       </c>
       <c r="P7">
-        <v>25.8</v>
+        <v>28.3</v>
       </c>
       <c r="Q7">
-        <v>76</v>
+        <v>75.3</v>
       </c>
       <c r="R7">
-        <v>26.9</v>
+        <v>29.7</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.55000000000000004">
@@ -1020,55 +1042,55 @@
         <v>5</v>
       </c>
       <c r="B8">
-        <v>46.5</v>
+        <v>47.5</v>
       </c>
       <c r="C8">
-        <v>70.099999999999994</v>
+        <v>67.8</v>
       </c>
       <c r="D8">
-        <v>34.799999999999997</v>
+        <v>36.6</v>
       </c>
       <c r="E8">
-        <v>48.4</v>
+        <v>50.1</v>
       </c>
       <c r="F8">
-        <v>97.6</v>
+        <v>92.8</v>
       </c>
       <c r="G8">
-        <v>0.12</v>
+        <v>0.4</v>
       </c>
       <c r="H8">
         <v>69</v>
       </c>
       <c r="I8">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J8">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K8">
         <v>36</v>
       </c>
       <c r="L8">
-        <v>107</v>
+        <v>359</v>
       </c>
       <c r="M8">
-        <v>4734</v>
+        <v>4574</v>
       </c>
       <c r="N8">
-        <v>63</v>
+        <v>77</v>
       </c>
       <c r="O8">
-        <v>66</v>
+        <v>151</v>
       </c>
       <c r="P8">
-        <v>46.5</v>
+        <v>45.4</v>
       </c>
       <c r="Q8">
-        <v>78.8</v>
+        <v>78.7</v>
       </c>
       <c r="R8">
-        <v>47.2</v>
+        <v>46.2</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.55000000000000004">
@@ -1076,55 +1098,55 @@
         <v>6</v>
       </c>
       <c r="B9">
-        <v>11.3</v>
+        <v>14.6</v>
       </c>
       <c r="C9">
-        <v>64.7</v>
+        <v>61.8</v>
       </c>
       <c r="D9">
-        <v>6.2</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="E9">
-        <v>9.1999999999999993</v>
+        <v>12.6</v>
       </c>
       <c r="F9">
-        <v>95.7</v>
+        <v>93.7</v>
       </c>
       <c r="G9">
-        <v>0.06</v>
+        <v>0.13</v>
       </c>
       <c r="H9">
         <v>107</v>
       </c>
       <c r="I9">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J9">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="K9">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="L9">
-        <v>47</v>
+        <v>96</v>
       </c>
       <c r="M9">
-        <v>10398</v>
+        <v>10011</v>
       </c>
       <c r="N9">
-        <v>36</v>
+        <v>199</v>
       </c>
       <c r="O9">
-        <v>39</v>
+        <v>206</v>
       </c>
       <c r="P9">
-        <v>8.5</v>
+        <v>10</v>
       </c>
       <c r="Q9">
-        <v>74.3</v>
+        <v>73.5</v>
       </c>
       <c r="R9">
-        <v>8.8000000000000007</v>
+        <v>11.7</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.55000000000000004">
@@ -1132,55 +1154,69 @@
         <v>7</v>
       </c>
       <c r="B10">
-        <v>25.4</v>
+        <v>29.8</v>
       </c>
       <c r="C10">
-        <v>56.4</v>
+        <v>60</v>
       </c>
       <c r="D10">
-        <v>16.399999999999999</v>
+        <v>19.8</v>
       </c>
       <c r="E10">
-        <v>28.1</v>
+        <v>30.9</v>
       </c>
       <c r="F10">
-        <v>96.7</v>
+        <v>93.4</v>
       </c>
       <c r="G10">
-        <v>0.2</v>
+        <v>0.45</v>
       </c>
       <c r="H10">
         <v>517</v>
       </c>
       <c r="I10">
+        <v>32</v>
+      </c>
+      <c r="J10">
+        <v>187</v>
+      </c>
+      <c r="K10">
+        <v>298</v>
+      </c>
+      <c r="L10">
+        <v>2405</v>
+      </c>
+      <c r="M10">
+        <v>76328</v>
+      </c>
+      <c r="N10">
+        <v>1374</v>
+      </c>
+      <c r="O10">
+        <v>2523</v>
+      </c>
+      <c r="P10" s="2">
+        <v>27.4</v>
+      </c>
+      <c r="Q10">
+        <v>77.5</v>
+      </c>
+      <c r="R10">
+        <v>28.7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" t="s">
         <v>25</v>
       </c>
-      <c r="J10">
-        <v>162</v>
-      </c>
-      <c r="K10">
-        <v>330</v>
-      </c>
-      <c r="L10">
-        <v>1064</v>
-      </c>
-      <c r="M10">
-        <v>79436</v>
-      </c>
-      <c r="N10">
-        <v>751</v>
-      </c>
-      <c r="O10">
-        <v>841</v>
-      </c>
-      <c r="P10" s="2">
-        <v>26.4</v>
-      </c>
-      <c r="Q10">
-        <v>78.099999999999994</v>
-      </c>
-      <c r="R10">
-        <v>27.1</v>
+      <c r="B12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.55000000000000004">
@@ -1188,16 +1224,28 @@
         <v>26</v>
       </c>
       <c r="B13" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C13" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="D13" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="E13" t="s">
-        <v>44</v>
+        <v>50</v>
+      </c>
+      <c r="F13" t="s">
+        <v>51</v>
+      </c>
+      <c r="G13" t="s">
+        <v>53</v>
+      </c>
+      <c r="H13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I13" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.55000000000000004">
@@ -1205,20 +1253,28 @@
         <v>0</v>
       </c>
       <c r="B14">
-        <v>93</v>
+        <v>0.3</v>
       </c>
       <c r="C14">
-        <v>4.7149999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="D14">
-        <v>93</v>
+        <v>0.3</v>
       </c>
       <c r="E14">
-        <v>4.7149999999999999</v>
+        <v>5</v>
       </c>
       <c r="F14">
-        <f>(D14-ground_truth!B2)/ground_truth!B2 * 100</f>
-        <v>40.909090909090914</v>
+        <v>2</v>
+      </c>
+      <c r="G14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>202</v>
+      </c>
+      <c r="I14">
+        <v>5.4233333333333302</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.55000000000000004">
@@ -1226,20 +1282,28 @@
         <v>1</v>
       </c>
       <c r="B15">
-        <v>389</v>
+        <v>0.3</v>
       </c>
       <c r="C15">
-        <v>14.9323809523809</v>
+        <v>0.5</v>
       </c>
       <c r="D15">
-        <v>389</v>
+        <v>0.3</v>
       </c>
       <c r="E15">
-        <v>14.9323809523809</v>
+        <v>5</v>
       </c>
       <c r="F15">
-        <f>(D15-ground_truth!B3)/ground_truth!B3 * 100</f>
-        <v>342.04545454545456</v>
+        <v>2</v>
+      </c>
+      <c r="G15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>836</v>
+      </c>
+      <c r="I15">
+        <v>16.760000000000002</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.55000000000000004">
@@ -1247,104 +1311,144 @@
         <v>2</v>
       </c>
       <c r="B16">
-        <v>95</v>
+        <v>0.3</v>
       </c>
       <c r="C16">
-        <v>2.42032622333751</v>
+        <v>0.5</v>
       </c>
       <c r="D16">
-        <v>95</v>
+        <v>0.3</v>
       </c>
       <c r="E16">
-        <v>2.42032622333751</v>
+        <v>5</v>
       </c>
       <c r="F16">
-        <f>(D16-ground_truth!B4)/ground_truth!B4 * 100</f>
-        <v>-26.356589147286826</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>2</v>
+      </c>
+      <c r="G16" t="b">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>223</v>
+      </c>
+      <c r="I16">
+        <v>2.78986402966625</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>3</v>
       </c>
       <c r="B17">
-        <v>106</v>
+        <v>0.3</v>
       </c>
       <c r="C17">
-        <v>5.0857142857142801</v>
+        <v>0.5</v>
       </c>
       <c r="D17">
-        <v>106</v>
+        <v>0.3</v>
       </c>
       <c r="E17">
-        <v>5.0857142857142801</v>
+        <v>5</v>
       </c>
       <c r="F17">
-        <f>(D17-ground_truth!B5)/ground_truth!B5 * 100</f>
-        <v>324</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>2</v>
+      </c>
+      <c r="G17" t="b">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>207</v>
+      </c>
+      <c r="I17">
+        <v>5.78095238095238</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>4</v>
       </c>
       <c r="B18">
-        <v>164</v>
+        <v>0.3</v>
       </c>
       <c r="C18">
-        <v>5.28440366972477</v>
+        <v>0.5</v>
       </c>
       <c r="D18">
-        <v>164</v>
+        <v>0.3</v>
       </c>
       <c r="E18">
-        <v>5.28440366972477</v>
+        <v>5</v>
       </c>
       <c r="F18">
-        <f>(D18-ground_truth!B6)/ground_truth!B6 * 100</f>
-        <v>187.71929824561403</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>2</v>
+      </c>
+      <c r="G18" t="b">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>309</v>
+      </c>
+      <c r="I18">
+        <v>6.3501529051987697</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>5</v>
       </c>
       <c r="B19">
-        <v>101</v>
+        <v>0.3</v>
       </c>
       <c r="C19">
-        <v>5.0522222222222197</v>
+        <v>0.5</v>
       </c>
       <c r="D19">
-        <v>101</v>
+        <v>0.3</v>
       </c>
       <c r="E19">
-        <v>5.0522222222222197</v>
+        <v>5</v>
       </c>
       <c r="F19">
-        <f>(D19-ground_truth!B7)/ground_truth!B7 * 100</f>
-        <v>46.376811594202898</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>2</v>
+      </c>
+      <c r="G19" t="b">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>225</v>
+      </c>
+      <c r="I19">
+        <v>5.51555555555555</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>6</v>
       </c>
       <c r="B20">
-        <v>70</v>
+        <v>0.3</v>
       </c>
       <c r="C20">
-        <v>1.93827160493827</v>
+        <v>0.5</v>
       </c>
       <c r="D20">
-        <v>70</v>
+        <v>0.3</v>
       </c>
       <c r="E20">
-        <v>1.93827160493827</v>
+        <v>5</v>
       </c>
       <c r="F20">
-        <f>(D20-ground_truth!B8)/ground_truth!B8 * 100</f>
-        <v>-34.579439252336449</v>
+        <v>2</v>
+      </c>
+      <c r="G20" t="b">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>259</v>
+      </c>
+      <c r="I20">
+        <v>2.3579109062980002</v>
       </c>
     </row>
   </sheetData>
@@ -1354,19 +1458,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2550A17C-7434-4E12-B770-FCC45E0A01A6}">
-  <dimension ref="A1:R21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8611D968-EEAD-4617-8B40-E1DBE56A0987}">
+  <dimension ref="A1:R20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="14.15625" customWidth="1"/>
+    <col min="6" max="6" width="5.3671875" customWidth="1"/>
+    <col min="7" max="7" width="12.47265625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" t="s">
-        <v>46</v>
-      </c>
+      <c r="A1" s="1"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
@@ -1424,154 +1531,616 @@
         <v>24</v>
       </c>
     </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>14.4</v>
+      </c>
+      <c r="C3">
+        <v>53.1</v>
+      </c>
+      <c r="D3">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="E3">
+        <v>15.1</v>
+      </c>
+      <c r="F3">
+        <v>96</v>
+      </c>
+      <c r="G3">
+        <v>0.19</v>
+      </c>
+      <c r="H3">
+        <v>54</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
+      </c>
+      <c r="J3">
+        <v>14</v>
+      </c>
+      <c r="K3">
+        <v>38</v>
+      </c>
+      <c r="L3">
+        <v>112</v>
+      </c>
+      <c r="M3">
+        <v>15144</v>
+      </c>
+      <c r="N3">
+        <v>66</v>
+      </c>
+      <c r="O3">
+        <v>85</v>
+      </c>
+      <c r="P3">
+        <v>14.1</v>
+      </c>
+      <c r="Q3">
+        <v>75.900000000000006</v>
+      </c>
+      <c r="R3">
+        <v>14.4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>26.1</v>
+      </c>
+      <c r="C4">
+        <v>52.7</v>
+      </c>
+      <c r="D4">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="E4">
+        <v>31.7</v>
+      </c>
+      <c r="F4">
+        <v>96.5</v>
+      </c>
+      <c r="G4">
+        <v>0.52</v>
+      </c>
+      <c r="H4">
+        <v>83</v>
+      </c>
+      <c r="I4">
+        <v>5</v>
+      </c>
+      <c r="J4">
+        <v>36</v>
+      </c>
+      <c r="K4">
+        <v>42</v>
+      </c>
+      <c r="L4">
+        <v>549</v>
+      </c>
+      <c r="M4">
+        <v>32460</v>
+      </c>
+      <c r="N4">
+        <v>317</v>
+      </c>
+      <c r="O4">
+        <v>335</v>
+      </c>
+      <c r="P4">
+        <v>29.9</v>
+      </c>
+      <c r="Q4">
+        <v>79.7</v>
+      </c>
+      <c r="R4">
+        <v>30.6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>29.8</v>
+      </c>
+      <c r="C5">
+        <v>67.7</v>
+      </c>
+      <c r="D5">
+        <v>19.100000000000001</v>
+      </c>
+      <c r="E5">
+        <v>27.2</v>
+      </c>
+      <c r="F5">
+        <v>96.2</v>
+      </c>
+      <c r="G5">
+        <v>0.09</v>
+      </c>
+      <c r="H5">
+        <v>125</v>
+      </c>
+      <c r="I5">
+        <v>4</v>
+      </c>
+      <c r="J5">
+        <v>42</v>
+      </c>
+      <c r="K5">
+        <v>79</v>
+      </c>
+      <c r="L5">
+        <v>73</v>
+      </c>
+      <c r="M5">
+        <v>4962</v>
+      </c>
+      <c r="N5">
+        <v>49</v>
+      </c>
+      <c r="O5">
+        <v>65</v>
+      </c>
+      <c r="P5">
+        <v>25.4</v>
+      </c>
+      <c r="Q5">
+        <v>77.3</v>
+      </c>
+      <c r="R5">
+        <v>26.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>42.6</v>
+      </c>
+      <c r="C6">
+        <v>65.099999999999994</v>
+      </c>
+      <c r="D6">
+        <v>31.7</v>
+      </c>
+      <c r="E6">
+        <v>46.6</v>
+      </c>
+      <c r="F6">
+        <v>95.8</v>
+      </c>
+      <c r="G6">
+        <v>0.21</v>
+      </c>
+      <c r="H6">
+        <v>25</v>
+      </c>
+      <c r="I6">
+        <v>4</v>
+      </c>
+      <c r="J6">
+        <v>16</v>
+      </c>
+      <c r="K6">
+        <v>5</v>
+      </c>
+      <c r="L6">
+        <v>108</v>
+      </c>
+      <c r="M6">
+        <v>2808</v>
+      </c>
+      <c r="N6">
+        <v>83</v>
+      </c>
+      <c r="O6">
+        <v>101</v>
+      </c>
+      <c r="P6">
+        <v>43</v>
+      </c>
+      <c r="Q6">
+        <v>74.900000000000006</v>
+      </c>
+      <c r="R6">
+        <v>44.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>18.7</v>
+      </c>
+      <c r="C7">
+        <v>42.6</v>
+      </c>
+      <c r="D7">
+        <v>11.9</v>
+      </c>
+      <c r="E7">
+        <v>27.5</v>
+      </c>
+      <c r="F7">
+        <v>98</v>
+      </c>
+      <c r="G7">
+        <v>0.1</v>
+      </c>
+      <c r="H7">
+        <v>54</v>
+      </c>
+      <c r="I7">
+        <v>2</v>
+      </c>
+      <c r="J7">
+        <v>16</v>
+      </c>
+      <c r="K7">
+        <v>36</v>
+      </c>
+      <c r="L7">
+        <v>68</v>
+      </c>
+      <c r="M7">
+        <v>8930</v>
+      </c>
+      <c r="N7">
+        <v>137</v>
+      </c>
+      <c r="O7">
+        <v>150</v>
+      </c>
+      <c r="P7">
+        <v>25.8</v>
+      </c>
+      <c r="Q7">
+        <v>76</v>
+      </c>
+      <c r="R7">
+        <v>26.9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>46.5</v>
+      </c>
+      <c r="C8">
+        <v>70.099999999999994</v>
+      </c>
+      <c r="D8">
+        <v>34.799999999999997</v>
+      </c>
+      <c r="E8">
+        <v>48.4</v>
+      </c>
+      <c r="F8">
+        <v>97.6</v>
+      </c>
+      <c r="G8">
+        <v>0.12</v>
+      </c>
+      <c r="H8">
+        <v>69</v>
+      </c>
+      <c r="I8">
+        <v>6</v>
+      </c>
+      <c r="J8">
+        <v>27</v>
+      </c>
+      <c r="K8">
+        <v>36</v>
+      </c>
+      <c r="L8">
+        <v>107</v>
+      </c>
+      <c r="M8">
+        <v>4734</v>
+      </c>
+      <c r="N8">
+        <v>63</v>
+      </c>
+      <c r="O8">
+        <v>66</v>
+      </c>
+      <c r="P8">
+        <v>46.5</v>
+      </c>
+      <c r="Q8">
+        <v>78.8</v>
+      </c>
+      <c r="R8">
+        <v>47.2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9">
+        <v>11.3</v>
+      </c>
+      <c r="C9">
+        <v>64.7</v>
+      </c>
+      <c r="D9">
+        <v>6.2</v>
+      </c>
+      <c r="E9">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="F9">
+        <v>95.7</v>
+      </c>
+      <c r="G9">
+        <v>0.06</v>
+      </c>
+      <c r="H9">
+        <v>107</v>
+      </c>
+      <c r="I9">
+        <v>2</v>
+      </c>
+      <c r="J9">
+        <v>11</v>
+      </c>
+      <c r="K9">
+        <v>94</v>
+      </c>
+      <c r="L9">
+        <v>47</v>
+      </c>
+      <c r="M9">
+        <v>10398</v>
+      </c>
+      <c r="N9">
+        <v>36</v>
+      </c>
+      <c r="O9">
+        <v>39</v>
+      </c>
+      <c r="P9">
+        <v>8.5</v>
+      </c>
+      <c r="Q9">
+        <v>74.3</v>
+      </c>
+      <c r="R9">
+        <v>8.8000000000000007</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10">
+        <v>25.4</v>
+      </c>
+      <c r="C10">
+        <v>56.4</v>
+      </c>
+      <c r="D10">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="E10">
+        <v>28.1</v>
+      </c>
+      <c r="F10">
+        <v>96.7</v>
+      </c>
+      <c r="G10">
+        <v>0.2</v>
+      </c>
+      <c r="H10">
+        <v>517</v>
+      </c>
+      <c r="I10">
+        <v>25</v>
+      </c>
+      <c r="J10">
+        <v>162</v>
+      </c>
+      <c r="K10">
+        <v>330</v>
+      </c>
+      <c r="L10">
+        <v>1064</v>
+      </c>
+      <c r="M10">
+        <v>79436</v>
+      </c>
+      <c r="N10">
+        <v>751</v>
+      </c>
+      <c r="O10">
+        <v>841</v>
+      </c>
+      <c r="P10" s="2">
+        <v>26.4</v>
+      </c>
+      <c r="Q10">
+        <v>78.099999999999994</v>
+      </c>
+      <c r="R10">
+        <v>27.1</v>
+      </c>
+    </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="3" t="s">
-        <v>25</v>
+      <c r="A13" t="s">
+        <v>26</v>
       </c>
       <c r="B13" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C13" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D13" t="s">
-        <v>40</v>
+        <v>43</v>
+      </c>
+      <c r="E13" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" t="s">
-        <v>29</v>
-      </c>
-      <c r="C14" t="s">
-        <v>30</v>
-      </c>
-      <c r="D14" t="s">
-        <v>31</v>
-      </c>
-      <c r="E14" t="s">
-        <v>32</v>
+        <v>0</v>
+      </c>
+      <c r="B14">
+        <v>93</v>
+      </c>
+      <c r="C14">
+        <v>4.7149999999999999</v>
+      </c>
+      <c r="D14">
+        <v>93</v>
+      </c>
+      <c r="E14">
+        <v>4.7149999999999999</v>
+      </c>
+      <c r="F14">
+        <f>(D14-ground_truth!B2)/ground_truth!B2 * 100</f>
+        <v>40.909090909090914</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>389</v>
       </c>
       <c r="C15">
-        <v>3</v>
+        <v>14.9323809523809</v>
       </c>
       <c r="D15">
-        <v>40</v>
+        <v>389</v>
       </c>
       <c r="E15">
-        <v>13.3333333333333</v>
+        <v>14.9323809523809</v>
+      </c>
+      <c r="F15">
+        <f>(D15-ground_truth!B3)/ground_truth!B3 * 100</f>
+        <v>342.04545454545456</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B16">
-        <v>1</v>
+        <v>95</v>
       </c>
       <c r="C16">
+        <v>2.42032622333751</v>
+      </c>
+      <c r="D16">
+        <v>95</v>
+      </c>
+      <c r="E16">
+        <v>2.42032622333751</v>
+      </c>
+      <c r="F16">
+        <f>(D16-ground_truth!B4)/ground_truth!B4 * 100</f>
+        <v>-26.356589147286826</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" t="s">
         <v>3</v>
       </c>
-      <c r="D16">
-        <v>126</v>
-      </c>
-      <c r="E16">
-        <v>3.0833333333333299</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" t="s">
-        <v>2</v>
-      </c>
       <c r="B17">
-        <v>1</v>
+        <v>106</v>
       </c>
       <c r="C17">
-        <v>3</v>
+        <v>5.0857142857142801</v>
       </c>
       <c r="D17">
-        <v>8</v>
+        <v>106</v>
       </c>
       <c r="E17">
-        <v>1.25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>5.0857142857142801</v>
+      </c>
+      <c r="F17">
+        <f>(D17-ground_truth!B5)/ground_truth!B5 * 100</f>
+        <v>324</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B18">
-        <v>1</v>
+        <v>164</v>
       </c>
       <c r="C18">
-        <v>3</v>
+        <v>5.28440366972477</v>
       </c>
       <c r="D18">
-        <v>27</v>
+        <v>164</v>
       </c>
       <c r="E18">
-        <v>1.88</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>5.28440366972477</v>
+      </c>
+      <c r="F18">
+        <f>(D18-ground_truth!B6)/ground_truth!B6 * 100</f>
+        <v>187.71929824561403</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B19">
-        <v>1</v>
+        <v>101</v>
       </c>
       <c r="C19">
-        <v>3</v>
+        <v>5.0522222222222197</v>
       </c>
       <c r="D19">
-        <v>54</v>
+        <v>101</v>
       </c>
       <c r="E19">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>5.0522222222222197</v>
+      </c>
+      <c r="F19">
+        <f>(D19-ground_truth!B7)/ground_truth!B7 * 100</f>
+        <v>46.376811594202898</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B20">
-        <v>1</v>
+        <v>70</v>
       </c>
       <c r="C20">
-        <v>3</v>
+        <v>1.93827160493827</v>
       </c>
       <c r="D20">
-        <v>25</v>
+        <v>70</v>
       </c>
       <c r="E20">
-        <v>1.9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" t="s">
-        <v>6</v>
-      </c>
-      <c r="B21">
-        <v>1</v>
-      </c>
-      <c r="C21">
-        <v>3</v>
-      </c>
-      <c r="D21">
-        <v>41</v>
-      </c>
-      <c r="E21">
-        <v>13.6666666666666</v>
+        <v>1.93827160493827</v>
+      </c>
+      <c r="F20">
+        <f>(D20-ground_truth!B8)/ground_truth!B8 * 100</f>
+        <v>-34.579439252336449</v>
       </c>
     </row>
   </sheetData>
@@ -1581,6 +2150,687 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2550A17C-7434-4E12-B770-FCC45E0A01A6}">
+  <dimension ref="A1:R21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="10.9453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N2" t="s">
+        <v>20</v>
+      </c>
+      <c r="O2" t="s">
+        <v>21</v>
+      </c>
+      <c r="P2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>23</v>
+      </c>
+      <c r="R2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>21.1</v>
+      </c>
+      <c r="C3">
+        <v>48</v>
+      </c>
+      <c r="D3">
+        <v>13.5</v>
+      </c>
+      <c r="E3">
+        <v>22.4</v>
+      </c>
+      <c r="F3">
+        <v>79.599999999999994</v>
+      </c>
+      <c r="G3">
+        <v>1.71</v>
+      </c>
+      <c r="H3">
+        <v>54</v>
+      </c>
+      <c r="I3">
+        <v>5</v>
+      </c>
+      <c r="J3">
+        <v>13</v>
+      </c>
+      <c r="K3">
+        <v>36</v>
+      </c>
+      <c r="L3">
+        <v>1024</v>
+      </c>
+      <c r="M3">
+        <v>13845</v>
+      </c>
+      <c r="N3">
+        <v>143</v>
+      </c>
+      <c r="O3">
+        <v>186</v>
+      </c>
+      <c r="P3">
+        <v>15.8</v>
+      </c>
+      <c r="Q3">
+        <v>75.900000000000006</v>
+      </c>
+      <c r="R3">
+        <v>16.600000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>29.2</v>
+      </c>
+      <c r="C4">
+        <v>39.299999999999997</v>
+      </c>
+      <c r="D4">
+        <v>23.2</v>
+      </c>
+      <c r="E4">
+        <v>43</v>
+      </c>
+      <c r="F4">
+        <v>72.8</v>
+      </c>
+      <c r="G4">
+        <v>7.3</v>
+      </c>
+      <c r="H4">
+        <v>83</v>
+      </c>
+      <c r="I4">
+        <v>8</v>
+      </c>
+      <c r="J4">
+        <v>42</v>
+      </c>
+      <c r="K4">
+        <v>33</v>
+      </c>
+      <c r="L4">
+        <v>7666</v>
+      </c>
+      <c r="M4">
+        <v>27086</v>
+      </c>
+      <c r="N4">
+        <v>435</v>
+      </c>
+      <c r="O4">
+        <v>612</v>
+      </c>
+      <c r="P4">
+        <v>26</v>
+      </c>
+      <c r="Q4">
+        <v>79.099999999999994</v>
+      </c>
+      <c r="R4">
+        <v>26.9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>32.5</v>
+      </c>
+      <c r="C5">
+        <v>56</v>
+      </c>
+      <c r="D5">
+        <v>22.9</v>
+      </c>
+      <c r="E5">
+        <v>34.1</v>
+      </c>
+      <c r="F5">
+        <v>83.6</v>
+      </c>
+      <c r="G5">
+        <v>0.54</v>
+      </c>
+      <c r="H5">
+        <v>125</v>
+      </c>
+      <c r="I5">
+        <v>3</v>
+      </c>
+      <c r="J5">
+        <v>60</v>
+      </c>
+      <c r="K5">
+        <v>62</v>
+      </c>
+      <c r="L5">
+        <v>455</v>
+      </c>
+      <c r="M5">
+        <v>4491</v>
+      </c>
+      <c r="N5">
+        <v>117</v>
+      </c>
+      <c r="O5">
+        <v>126</v>
+      </c>
+      <c r="P5">
+        <v>25.7</v>
+      </c>
+      <c r="Q5">
+        <v>76.099999999999994</v>
+      </c>
+      <c r="R5">
+        <v>27.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>41.7</v>
+      </c>
+      <c r="C6">
+        <v>49.1</v>
+      </c>
+      <c r="D6">
+        <v>36.299999999999997</v>
+      </c>
+      <c r="E6">
+        <v>56.2</v>
+      </c>
+      <c r="F6">
+        <v>76.2</v>
+      </c>
+      <c r="G6">
+        <v>1.76</v>
+      </c>
+      <c r="H6">
+        <v>25</v>
+      </c>
+      <c r="I6">
+        <v>4</v>
+      </c>
+      <c r="J6">
+        <v>17</v>
+      </c>
+      <c r="K6">
+        <v>4</v>
+      </c>
+      <c r="L6">
+        <v>924</v>
+      </c>
+      <c r="M6">
+        <v>2301</v>
+      </c>
+      <c r="N6">
+        <v>94</v>
+      </c>
+      <c r="O6">
+        <v>112</v>
+      </c>
+      <c r="P6">
+        <v>36.9</v>
+      </c>
+      <c r="Q6">
+        <v>74.3</v>
+      </c>
+      <c r="R6">
+        <v>38.6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>28.3</v>
+      </c>
+      <c r="C7">
+        <v>45.2</v>
+      </c>
+      <c r="D7">
+        <v>20.6</v>
+      </c>
+      <c r="E7">
+        <v>36.799999999999997</v>
+      </c>
+      <c r="F7">
+        <v>80.7</v>
+      </c>
+      <c r="G7">
+        <v>1.66</v>
+      </c>
+      <c r="H7">
+        <v>54</v>
+      </c>
+      <c r="I7">
+        <v>5</v>
+      </c>
+      <c r="J7">
+        <v>19</v>
+      </c>
+      <c r="K7">
+        <v>30</v>
+      </c>
+      <c r="L7">
+        <v>1084</v>
+      </c>
+      <c r="M7">
+        <v>7783</v>
+      </c>
+      <c r="N7">
+        <v>151</v>
+      </c>
+      <c r="O7">
+        <v>244</v>
+      </c>
+      <c r="P7">
+        <v>26.8</v>
+      </c>
+      <c r="Q7">
+        <v>75.5</v>
+      </c>
+      <c r="R7">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>41.3</v>
+      </c>
+      <c r="C8">
+        <v>51.8</v>
+      </c>
+      <c r="D8">
+        <v>34.4</v>
+      </c>
+      <c r="E8">
+        <v>53.7</v>
+      </c>
+      <c r="F8">
+        <v>81</v>
+      </c>
+      <c r="G8">
+        <v>1.28</v>
+      </c>
+      <c r="H8">
+        <v>69</v>
+      </c>
+      <c r="I8">
+        <v>9</v>
+      </c>
+      <c r="J8">
+        <v>24</v>
+      </c>
+      <c r="K8">
+        <v>36</v>
+      </c>
+      <c r="L8">
+        <v>1154</v>
+      </c>
+      <c r="M8">
+        <v>4243</v>
+      </c>
+      <c r="N8">
+        <v>75</v>
+      </c>
+      <c r="O8">
+        <v>83</v>
+      </c>
+      <c r="P8">
+        <v>40.4</v>
+      </c>
+      <c r="Q8">
+        <v>79</v>
+      </c>
+      <c r="R8">
+        <v>41.2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9">
+        <v>25.9</v>
+      </c>
+      <c r="C9">
+        <v>64</v>
+      </c>
+      <c r="D9">
+        <v>16.3</v>
+      </c>
+      <c r="E9">
+        <v>20.3</v>
+      </c>
+      <c r="F9">
+        <v>79.900000000000006</v>
+      </c>
+      <c r="G9">
+        <v>0.78</v>
+      </c>
+      <c r="H9">
+        <v>107</v>
+      </c>
+      <c r="I9">
+        <v>7</v>
+      </c>
+      <c r="J9">
+        <v>31</v>
+      </c>
+      <c r="K9">
+        <v>69</v>
+      </c>
+      <c r="L9">
+        <v>586</v>
+      </c>
+      <c r="M9">
+        <v>9125</v>
+      </c>
+      <c r="N9">
+        <v>87</v>
+      </c>
+      <c r="O9">
+        <v>143</v>
+      </c>
+      <c r="P9">
+        <v>14.4</v>
+      </c>
+      <c r="Q9">
+        <v>73.5</v>
+      </c>
+      <c r="R9">
+        <v>15.2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10">
+        <v>29.7</v>
+      </c>
+      <c r="C10">
+        <v>45</v>
+      </c>
+      <c r="D10">
+        <v>22.2</v>
+      </c>
+      <c r="E10">
+        <v>37.6</v>
+      </c>
+      <c r="F10">
+        <v>76.3</v>
+      </c>
+      <c r="G10">
+        <v>2.4300000000000002</v>
+      </c>
+      <c r="H10">
+        <v>517</v>
+      </c>
+      <c r="I10">
+        <v>41</v>
+      </c>
+      <c r="J10">
+        <v>206</v>
+      </c>
+      <c r="K10">
+        <v>270</v>
+      </c>
+      <c r="L10">
+        <v>12893</v>
+      </c>
+      <c r="M10">
+        <v>68874</v>
+      </c>
+      <c r="N10">
+        <v>1102</v>
+      </c>
+      <c r="O10">
+        <v>1506</v>
+      </c>
+      <c r="P10" s="2">
+        <v>24.9</v>
+      </c>
+      <c r="Q10">
+        <v>77.5</v>
+      </c>
+      <c r="R10">
+        <v>25.9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>3</v>
+      </c>
+      <c r="D15">
+        <v>40</v>
+      </c>
+      <c r="E15">
+        <v>13.3333333333333</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>3</v>
+      </c>
+      <c r="D16">
+        <v>126</v>
+      </c>
+      <c r="E16">
+        <v>3.0833333333333299</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>3</v>
+      </c>
+      <c r="D17">
+        <v>8</v>
+      </c>
+      <c r="E17">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
+      </c>
+      <c r="D18">
+        <v>27</v>
+      </c>
+      <c r="E18">
+        <v>1.88</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>3</v>
+      </c>
+      <c r="D19">
+        <v>54</v>
+      </c>
+      <c r="E19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>3</v>
+      </c>
+      <c r="D20">
+        <v>25</v>
+      </c>
+      <c r="E20">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>3</v>
+      </c>
+      <c r="D21">
+        <v>41</v>
+      </c>
+      <c r="E21">
+        <v>13.6666666666666</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" xr:uid="{C6701484-1009-43A5-B8A2-A5BE588446E0}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{016F5681-380E-497D-A5D0-C78F88FBF6E7}">
   <dimension ref="A1:R20"/>
   <sheetViews>
@@ -1591,7 +2841,7 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="11.05078125" customWidth="1"/>
-    <col min="7" max="7" width="19.26171875" customWidth="1"/>
+    <col min="7" max="7" width="11.1015625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.55000000000000004">
@@ -2329,12 +3579,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9515722-321E-4F21-8A44-93AC984BEED1}">
   <dimension ref="A1:R20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A10"/>
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2842,7 +4092,7 @@
       <c r="O10">
         <v>983</v>
       </c>
-      <c r="P10">
+      <c r="P10" s="2">
         <v>23.7</v>
       </c>
       <c r="Q10">
@@ -3075,12 +4325,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62791F90-C7BC-4273-BF71-38B690B0C6D5}">
   <dimension ref="A1:R20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3588,7 +4838,7 @@
       <c r="O10">
         <v>972</v>
       </c>
-      <c r="P10">
+      <c r="P10" s="2">
         <v>21.3</v>
       </c>
       <c r="Q10">
@@ -3835,7 +5085,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{100D8D13-5042-4D32-870C-476FD1E164DC}">
   <dimension ref="A1:R20"/>
   <sheetViews>

</xml_diff>